<commit_message>
Adding HPI info to data dict
</commit_message>
<xml_diff>
--- a/cs5010_Dict_DRAFTv1_100120.xlsx
+++ b/cs5010_Dict_DRAFTv1_100120.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newma\Data_v1\cs5010\LifeOfBrian-USHousing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana McSpadden\Documents\UVaCode\Python\LifeOfBrian-USHousing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E841DD3E-2788-4704-AE46-6D0CFEF05BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C888669C-11F0-49BA-90A1-1C637BCEFAC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
+    <workbookView xWindow="32745" yWindow="780" windowWidth="23505" windowHeight="12405" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="77">
   <si>
     <t>Source</t>
   </si>
@@ -150,6 +150,120 @@
   </si>
   <si>
     <t xml:space="preserve">CS5010 - LifeOfBrian </t>
+  </si>
+  <si>
+    <t>hpi_type</t>
+  </si>
+  <si>
+    <t>Quant</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>HPI_master.csv</t>
+  </si>
+  <si>
+    <t>FHFA.gov</t>
+  </si>
+  <si>
+    <t>traditional, developmental, distress-free, non-metro. The traditional, purchase-only, seasonally adjusted HPI is the index reported typically in press releases.</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>hpi_flavor</t>
+  </si>
+  <si>
+    <t>purchase-only, all-transactions, expanded-data: three main types of FHFA HPIs and they differ by their underlying data (not the statistical techniques creating the indexes). Only the all-transactions data are published before 1991.</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>Quant, Categorical, Filter</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t># Values</t>
+  </si>
+  <si>
+    <t>monthly, quarterly: time scale of resulting value</t>
+  </si>
+  <si>
+    <t>place_name</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>quarterly</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>level of geography: USA or Census Division, State, MSA, Puerto Rico</t>
+  </si>
+  <si>
+    <t>US, Census Division, State MSA, Puerto Rico (metropolitan statistical area)</t>
+  </si>
+  <si>
+    <t>MSA</t>
+  </si>
+  <si>
+    <t>Examples: East North Central Division; Alabama; Abilene, TX</t>
+  </si>
+  <si>
+    <t>USA Census Division</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>Year for HPI value</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>1 = annual, 1 - 4 quarterly, 1 - 12 monthly</t>
+  </si>
+  <si>
+    <t>Categorical/Filter</t>
+  </si>
+  <si>
+    <t>Annual, Quarter, Month</t>
+  </si>
+  <si>
+    <t>index_nsa</t>
+  </si>
+  <si>
+    <t>Housing Price Index - Not Seasonally Adjusted</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Avg Price Change</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>index_sa</t>
+  </si>
+  <si>
+    <t>Housing Price Index - Seasonally Adjusted</t>
   </si>
 </sst>
 </file>
@@ -214,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -234,6 +348,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,45 +666,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE930BE5-76EF-4DE3-A62A-9FA65577EC5F}">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="18" max="18" width="20.44140625" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
@@ -595,10 +715,10 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
@@ -612,49 +732,55 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -668,49 +794,55 @@
         <v>24</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="6">
+      <c r="I6" s="6">
         <v>36526</v>
       </c>
-      <c r="H6" s="6">
+      <c r="J6" s="6">
         <v>42705</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="5">
+      <c r="M6" s="5">
         <v>0</v>
       </c>
-      <c r="L6" s="5">
+      <c r="N6" s="5">
         <v>6424</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="R6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="T6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -724,229 +856,603 @@
         <v>24</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="9">
+      <c r="I7" s="9">
         <v>36526</v>
       </c>
-      <c r="H7" s="9">
+      <c r="J7" s="9">
         <v>36861</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="8">
+      <c r="M7" s="8">
         <v>0</v>
       </c>
-      <c r="L7" s="8">
+      <c r="N7" s="8">
         <v>23285</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="Q7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="R7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="S7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="T7" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J8" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="8">
+        <v>3</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J9" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="8">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J10" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="8">
+        <v>4</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J11" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="8">
+        <v>466</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J12" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="8">
+        <v>46</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1975</v>
+      </c>
+      <c r="J13" s="8">
+        <v>2020</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="8">
+        <v>1975</v>
+      </c>
+      <c r="N13" s="8">
+        <v>2020</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="8">
+        <v>12</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J14" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="8">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
+        <v>12</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J15" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="8">
+        <v>18.34</v>
+      </c>
+      <c r="N15" s="8">
+        <v>947.63</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="9">
+        <v>27395</v>
+      </c>
+      <c r="J16" s="9">
+        <v>43983</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="M16" s="8">
+        <v>70.650000000000006</v>
+      </c>
+      <c r="N16" s="8">
+        <v>584.77</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -965,8 +1471,10 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -985,8 +1493,10 @@
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1005,8 +1515,10 @@
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1025,8 +1537,10 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1045,8 +1559,10 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1065,8 +1581,10 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1085,8 +1603,10 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1105,8 +1625,10 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1125,8 +1647,10 @@
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1145,8 +1669,10 @@
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1165,8 +1691,10 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1185,8 +1713,10 @@
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1205,8 +1735,10 @@
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1225,8 +1757,10 @@
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1245,8 +1779,10 @@
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1265,8 +1801,10 @@
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1285,8 +1823,10 @@
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1305,6 +1845,8 @@
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>